<commit_message>
changes requested by editors
</commit_message>
<xml_diff>
--- a/data/supplementary_data/SupplementaryDataset1.xlsx
+++ b/data/supplementary_data/SupplementaryDataset1.xlsx
@@ -21,14 +21,14 @@
       <rPr>
         <b val="true"/>
       </rPr>
-      <t xml:space="preserve">Supplementary Dataset 1.</t>
+      <t xml:space="preserve">Supplementary Dataset S1.</t>
     </r>
     <r>
       <t xml:space="preserve"> Enrichment of insulator fragment constructs.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Known insulators were split into partially overlapping 170-bp fragments. The insulator fragments were cloned in the forward or reverse orientation between a 35S, AB80, or Cab-1 enhancer and a 35S minimal promoter driving the expression of a barcoded GFP reporter gene. Constructs without an enhancer (none) but with insulator fragments were also created. All insulator fragment constructs were pooled and subjected to Plant STARR-seq in tobacco leaves (tobacco) and maize protoplasts (maize). Reporter mRNA enrichment was normalized to a control construct without an enhancer or insulator (noEnh; log2 set to 0).</t>
+    <t xml:space="preserve">Known insulators were split into partially overlapping 170-bp fragments. The insulator fragments were cloned in the forward or reverse orientation between a 35S, AB80, or Cab-1 enhancer and a 35S minimal promoter driving the expression of a barcoded GFP reporter gene. Constructs without an enhancer (none) but with insulator fragments were also created. All insulator fragment constructs were pooled and subjected to Plant STARR-seq in N. benthamiana leaves (tobacco) and maize protoplasts (maize). Reporter mRNA enrichment was normalized to a control construct without an enhancer or insulator (noEnh; log2 set to 0).</t>
   </si>
   <si>
     <t xml:space="preserve">enhancer</t>

</xml_diff>